<commit_message>
humidity, pressure, feels_like, temperature icons + values
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="101">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -285,6 +285,39 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obecnie:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odczuwalna:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small_font</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">owm_style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°C0123456789.%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odczuw.:</t>
   </si>
 </sst>
 </file>
@@ -1527,7 +1560,7 @@
         <v>64</v>
       </c>
       <c r="D4">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1561,17 +1594,19 @@
         <v>64</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="H5"/>
-      <c r="I5"/>
+      <c r="I5" t="s">
+        <v>98</v>
+      </c>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
         <v>1</v>
@@ -1588,7 +1623,26 @@
       <c r="P5" s="10"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="I6"/>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6"/>
+      <c r="I6" t="s">
+        <v>98</v>
+      </c>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
         <v>2</v>
@@ -1605,6 +1659,27 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J7"/>
       <c r="L7" s="7" t="s">
         <v>15</v>
       </c>
@@ -1790,7 +1865,7 @@
         <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
         <v>55</v>
@@ -1821,21 +1896,40 @@
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F8" t="s">
         <v>56</v>
       </c>
     </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10"/>
+    <row r="11"/>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
wind_speed, cityname, weather desc
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="103">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -318,6 +318,12 @@
   </si>
   <si>
     <t xml:space="preserve">Odczuw.:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z,0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°.%/</t>
   </si>
 </sst>
 </file>
@@ -1601,11 +1607,11 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H5"/>
       <c r="I5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
@@ -1637,11 +1643,11 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
@@ -1673,11 +1679,11 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H7"/>
       <c r="I7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J7"/>
       <c r="L7" s="7" t="s">

</xml_diff>

<commit_message>
visibility, temperature inside, optimized pngs
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="113">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -345,6 +345,15 @@
   </si>
   <si>
     <t xml:space="preserve">°. %/ąęćółńżź </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp. wewnątrz:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp. wewnątrz</t>
   </si>
 </sst>
 </file>
@@ -1927,16 +1936,16 @@
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
         <v>56</v>
@@ -1944,7 +1953,7 @@
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
         <v>97</v>
@@ -1953,7 +1962,7 @@
         <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F8" t="s">
         <v>56</v>
@@ -1961,16 +1970,16 @@
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="F9" t="s">
         <v>56</v>
@@ -1978,16 +1987,16 @@
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="F10" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
keyboard finished project cleanup
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3041" uniqueCount="134">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -354,6 +354,69 @@
   </si>
   <si>
     <t xml:space="preserve">Temp. wewnątrz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RobotoCondensed-Regular.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!”"#*%&amp;()'$+-@_, .:;?/~±×÷•º`´{}©£€^®¥_=[]¡¢|\¿&gt;&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnteredText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;placeholder&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AlphaMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button_labels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazwa miasta:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wpisz co</t>
   </si>
 </sst>
 </file>
@@ -1769,6 +1832,29 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16">
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9"/>
       <c r="L9" s="11" t="s">
         <v>14</v>
       </c>
@@ -1786,6 +1872,29 @@
       </c>
     </row>
     <row r="10" spans="2:16">
+      <c r="B10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10"/>
       <c r="L10" s="11" t="s">
         <v>36</v>
       </c>
@@ -1801,9 +1910,47 @@
       <c r="P10" s="14"/>
     </row>
     <row r="11" spans="2:16">
+      <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:16">
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
       <c r="M12" s="16" t="s">
         <v>35</v>
       </c>
@@ -2002,7 +2149,125 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11"/>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">

</xml_diff>